<commit_message>
Dodana stran s kostumskimi podobami.
Co-authored-by: BarbaraPal <BarbaraPal@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Data/podatki/garderoba.xlsx
+++ b/Data/podatki/garderoba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majaa\Documents\FMF\OPB\OPB-organizacija-garderobe-folklornega-dru-tva\Data\podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A54579-5229-488C-B369-CC1A5351CA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF64C4E-5239-4757-9697-4A2EFDA0A742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10755" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="10" xr2:uid="{F6837F49-E7CC-4935-A88F-4A71D4516CA1}"/>
+    <workbookView xWindow="-10755" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F6837F49-E7CC-4935-A88F-4A71D4516CA1}"/>
   </bookViews>
   <sheets>
     <sheet name="OpravaKostumskePodobe" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="161">
   <si>
     <t>ImeKostumskePodobe</t>
   </si>
@@ -513,9 +513,6 @@
     <t>Moznost</t>
   </si>
   <si>
-    <t>ena plesalka ima namesto rute venček (mama); ruta vezana nazaj</t>
-  </si>
-  <si>
     <t>ruta vezana naprej ("bonbonček") ali nazaj</t>
   </si>
   <si>
@@ -523,6 +520,15 @@
   </si>
   <si>
     <t>ZaporednaSt</t>
+  </si>
+  <si>
+    <t>mama</t>
+  </si>
+  <si>
+    <t>ruta vezana nazaj</t>
+  </si>
+  <si>
+    <t>na glavi nosi venček; frizura: nizka figa</t>
   </si>
 </sst>
 </file>
@@ -975,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC16BC7-4F48-4819-9CF6-7D54A62DAC2F}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,7 +1020,7 @@
         <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1036,7 +1042,7 @@
         <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1058,7 +1064,7 @@
         <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1067,6 +1073,20 @@
       </c>
       <c r="B7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1460,7 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FFAE8F-B0AF-404A-9B63-946834018B8D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
@@ -1781,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC0CFA0-C80A-41AB-B963-B4B83B4E6529}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2290,6 +2310,120 @@
         <v>4</v>
       </c>
       <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
         <v>0</v>
       </c>
     </row>
@@ -2620,7 +2754,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2645,7 +2779,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -3956,7 +4090,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -4867,7 +5001,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Zadnji vnosi podatkov in priprava na oddajo.
Co-authored-by: BarbaraPal <BarbaraPal@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Data/podatki/garderoba.xlsx
+++ b/Data/podatki/garderoba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majaa\Documents\FMF\OPB\OPB-organizacija-garderobe-folklornega-dru-tva\Data\podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC79C50-C2FA-4433-B9E1-7796C56860E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735A28C3-2AAF-497E-8B51-10CB651D2D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10755" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F6837F49-E7CC-4935-A88F-4A71D4516CA1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{F6837F49-E7CC-4935-A88F-4A71D4516CA1}"/>
   </bookViews>
   <sheets>
     <sheet name="OpravaKostumskePodobe" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="194">
   <si>
     <t>ImeKostumskePodobe</t>
   </si>
@@ -255,9 +255,6 @@
     <t>moder enobarven</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>modra z zelenim vzorcem</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>rdeča</t>
   </si>
   <si>
-    <t>nezašit naborek</t>
-  </si>
-  <si>
     <t>zelen črtast</t>
   </si>
   <si>
@@ -607,6 +601,33 @@
   </si>
   <si>
     <t>PokrajinaVrste</t>
+  </si>
+  <si>
+    <t>ozkokrajni klobuk</t>
+  </si>
+  <si>
+    <t>telovnik</t>
+  </si>
+  <si>
+    <t>srajca</t>
+  </si>
+  <si>
+    <t>hlače</t>
+  </si>
+  <si>
+    <t>nizki škornji</t>
+  </si>
+  <si>
+    <t>žametni telovnik</t>
+  </si>
+  <si>
+    <t>Gorenjska</t>
+  </si>
+  <si>
+    <t>venček</t>
+  </si>
+  <si>
+    <t>strgan naborek</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1083,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1075,16 +1096,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1092,7 +1113,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1101,15 +1122,15 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1117,10 +1138,13 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1129,15 +1153,15 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1145,10 +1169,13 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1157,15 +1184,15 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1176,7 +1203,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1185,10 +1212,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1198,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B0E11-126C-4051-9668-106582B9C775}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1217,22 +1244,22 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1243,7 +1270,7 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1254,13 +1281,13 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -1277,7 +1304,7 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1288,13 +1315,13 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -1311,13 +1338,13 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1334,13 +1361,13 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -1357,7 +1384,7 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1368,13 +1395,13 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -1391,13 +1418,13 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -1414,13 +1441,13 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
@@ -1437,7 +1464,7 @@
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1448,13 +1475,13 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
@@ -1471,7 +1498,7 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1482,7 +1509,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1493,10 +1520,10 @@
         <v>37</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1504,10 +1531,10 @@
         <v>38</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1515,10 +1542,10 @@
         <v>38</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1526,10 +1553,10 @@
         <v>38</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1537,10 +1564,10 @@
         <v>39</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1548,10 +1575,10 @@
         <v>39</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1559,10 +1586,10 @@
         <v>40</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1570,7 +1597,165 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>42</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="9">
+        <v>44857</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>43</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>43</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="9">
+        <v>44490</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>43</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="9">
+        <v>43020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>44</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>44</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>44</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="9">
+        <v>43020</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>45</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>45</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>46</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +1768,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1597,39 +1782,39 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>138</v>
-      </c>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" t="s">
-        <v>140</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="12">
         <v>44993</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -1640,19 +1825,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" s="12">
         <v>44928</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -1663,19 +1848,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="12">
         <v>44928</v>
       </c>
       <c r="E4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1686,19 +1871,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D5" s="12">
         <v>44999</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -1709,19 +1894,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D6" s="12">
         <v>44999</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1732,19 +1917,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D7" s="12">
         <v>45049</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -1755,19 +1940,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" s="12">
         <v>45043</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
@@ -1778,19 +1963,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D9" s="12">
         <v>44979</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -1801,19 +1986,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D10" s="12">
         <v>45049</v>
       </c>
       <c r="E10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
@@ -1824,19 +2009,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D11" s="12">
         <v>44979</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -1847,19 +2032,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D12" s="12">
         <v>45043</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
@@ -1870,19 +2055,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D13" s="12">
         <v>44960</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -1903,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC0CFA0-C80A-41AB-B963-B4B83B4E6529}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1921,27 +2106,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1958,7 +2143,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1975,7 +2160,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1992,7 +2177,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -2009,7 +2194,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -2029,7 +2214,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -2049,7 +2234,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -2069,7 +2254,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -2089,7 +2274,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -2109,7 +2294,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -2126,7 +2311,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -2143,7 +2328,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -2163,7 +2348,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -2183,7 +2368,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -2203,7 +2388,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -2223,7 +2408,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -2243,7 +2428,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2260,7 +2445,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2277,7 +2462,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2297,7 +2482,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2317,7 +2502,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2337,7 +2522,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2357,7 +2542,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2377,7 +2562,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2397,7 +2582,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2417,7 +2602,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -2434,7 +2619,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -2451,7 +2636,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -2471,7 +2656,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -2491,7 +2676,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -2511,7 +2696,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -2526,6 +2711,200 @@
         <v>4</v>
       </c>
       <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>185</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" t="s">
+        <v>187</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42">
         <v>0</v>
       </c>
     </row>
@@ -2536,21 +2915,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166594E8-78FC-4A86-B145-BEDF23428F05}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -2562,7 +2942,7 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2576,7 +2956,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2587,10 +2967,10 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2601,10 +2981,10 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2615,10 +2995,10 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2635,7 +3015,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2652,7 +3032,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2669,7 +3049,7 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2686,7 +3066,7 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2700,10 +3080,10 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2720,7 +3100,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2737,7 +3117,7 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2754,7 +3134,7 @@
         <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2771,7 +3151,7 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -2785,10 +3165,10 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <v>-1</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -2802,10 +3182,10 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2819,10 +3199,10 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2836,10 +3216,10 @@
         <v>4</v>
       </c>
       <c r="D18">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2853,10 +3233,10 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2870,10 +3250,10 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2887,10 +3267,10 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -2904,10 +3284,160 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>188</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2919,10 +3449,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB52316-63FE-4923-8376-720F26AF2030}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2938,7 +3468,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -2947,7 +3477,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -3275,7 +3805,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="7">
         <v>98</v>
@@ -3298,7 +3828,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="7">
         <v>100</v>
@@ -3321,7 +3851,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17">
         <v>103</v>
@@ -3571,7 +4101,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F28">
         <v>96</v>
@@ -3617,7 +4147,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F30">
         <v>98</v>
@@ -3686,7 +4216,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33">
         <v>95</v>
@@ -3709,16 +4239,16 @@
         <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34">
         <v>103</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -3735,7 +4265,7 @@
         <v>8</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35">
         <v>94</v>
@@ -3758,7 +4288,7 @@
         <v>9</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F36">
         <v>94</v>
@@ -3804,7 +4334,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -3824,7 +4354,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -3844,7 +4374,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -3864,7 +4394,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -3884,7 +4414,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -3904,7 +4434,7 @@
         <v>6</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -3924,7 +4454,7 @@
         <v>7</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -3944,13 +4474,13 @@
         <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -3961,34 +4491,17 @@
         <v>4</v>
       </c>
       <c r="D46" s="6">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>69</v>
+        <v>10</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="6">
-        <v>10</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F48" s="8"/>
@@ -4016,9 +4529,6 @@
     </row>
     <row r="56" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F57" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4032,8 +4542,8 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4049,7 +4559,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -4058,7 +4568,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -4669,7 +5179,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F21">
         <v>38</v>
@@ -4698,7 +5208,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F22">
         <v>42</v>
@@ -4960,7 +5470,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -4969,13 +5479,13 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
         <v>35</v>
@@ -5024,7 +5534,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F3">
         <v>148</v>
@@ -5047,7 +5557,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F4">
         <v>144</v>
@@ -5070,7 +5580,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F5">
         <v>143</v>
@@ -5093,7 +5603,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F6">
         <v>141</v>
@@ -5139,7 +5649,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8">
         <v>136</v>
@@ -5162,7 +5672,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9">
         <v>132</v>
@@ -5185,7 +5695,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10">
         <v>132</v>
@@ -5208,7 +5718,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11">
         <v>130</v>
@@ -5239,7 +5749,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -5248,7 +5758,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
         <v>36</v>
@@ -5408,7 +5918,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5421,19 +5931,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
         <v>32</v>
@@ -5448,21 +5958,21 @@
         <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -5492,13 +6002,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -5528,13 +6038,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -5564,13 +6074,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -5600,13 +6110,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -5636,13 +6146,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -5672,13 +6182,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -5708,13 +6218,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -5744,13 +6254,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -5777,13 +6287,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -5810,13 +6320,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -5843,13 +6353,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -5876,13 +6386,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -5909,13 +6419,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -5942,13 +6452,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -5975,13 +6485,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -6013,10 +6523,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971F9DE0-24A3-439F-A03A-7C8B852B112B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6026,7 +6536,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
@@ -6034,12 +6544,17 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>